<commit_message>
v0.1: Updated profiles for better results
</commit_message>
<xml_diff>
--- a/Docs/Profiles.xlsx
+++ b/Docs/Profiles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\reflow-oven\Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\reflow-controller\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FC1EEC-FA68-4CF4-9473-53A2656D298A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984D8B35-1DE4-4981-82AE-4042B46453AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10670" xr2:uid="{3BB66555-8BBA-44F8-85BE-C703FDF9F232}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" xr2:uid="{3BB66555-8BBA-44F8-85BE-C703FDF9F232}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -413,16 +422,16 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>170</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>260</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>290</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>390</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1697,16 +1706,16 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>170</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>260</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>290</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>390</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4094,7 +4103,7 @@
   <dimension ref="B1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4155,20 +4164,20 @@
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="12"/>
       <c r="C6" s="6">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="D6" s="6">
         <v>180</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" ref="E6:E23" si="0">(D6-D5)/(C6-C5)</f>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" s="12"/>
       <c r="C7" s="6">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="D7" s="6">
         <v>250</v>
@@ -4181,7 +4190,7 @@
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" s="12"/>
       <c r="C8" s="6">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="D8" s="6">
         <v>250</v>
@@ -4194,7 +4203,7 @@
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="12"/>
       <c r="C9" s="6">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="D9" s="6">
         <v>50</v>

</xml_diff>